<commit_message>
Updated gitignore and Math is Fun
</commit_message>
<xml_diff>
--- a/Modules/ITD/Week 1/Math is Fun.xlsx
+++ b/Modules/ITD/Week 1/Math is Fun.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NP\Semesters\2021_OCT\ITD\Student Repo\IMYear2.2\Modules\ITD\Week 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0999E055-B242-4203-BB64-83F20DFCAE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C30B25F-43AD-4076-8024-BCC07AD349A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{03D92545-E4C8-4BA6-B9A5-B71E5C481EEB}"/>
+    <workbookView xWindow="-11250" yWindow="2100" windowWidth="21600" windowHeight="14970" xr2:uid="{03D92545-E4C8-4BA6-B9A5-B71E5C481EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>3n+2=2n+4</t>
   </si>
@@ -78,87 +78,9 @@
     <t>9y−15=8y−12</t>
   </si>
   <si>
-    <t>AARON</t>
-  </si>
-  <si>
-    <t>WEI XIANG</t>
-  </si>
-  <si>
-    <t>BRYAN</t>
-  </si>
-  <si>
-    <t>CHARLENE</t>
-  </si>
-  <si>
-    <t>NICHOLAS</t>
-  </si>
-  <si>
-    <t>CHRISTIAN</t>
-  </si>
-  <si>
-    <t>KAH MIN</t>
-  </si>
-  <si>
-    <t>DARRENCE</t>
-  </si>
-  <si>
-    <t>CHER WEI</t>
-  </si>
-  <si>
-    <t>JASLYN</t>
-  </si>
-  <si>
-    <t>KIRDESH</t>
-  </si>
-  <si>
-    <t>MARCUS</t>
-  </si>
-  <si>
-    <t>JIAYI</t>
-  </si>
-  <si>
-    <t>LINDSAY</t>
-  </si>
-  <si>
-    <t>KANG XUAN</t>
-  </si>
-  <si>
-    <t>MEAGAN</t>
-  </si>
-  <si>
-    <t>JONATHAN</t>
-  </si>
-  <si>
-    <t>DAN</t>
-  </si>
-  <si>
-    <t>LIN</t>
-  </si>
-  <si>
-    <t>REBECCA</t>
-  </si>
-  <si>
-    <t>ROYDEN</t>
-  </si>
-  <si>
-    <t>DARRIK</t>
-  </si>
-  <si>
-    <t>ZAVIER</t>
-  </si>
-  <si>
     <t>6w−2=5w+3</t>
   </si>
   <si>
-    <t>3n+5=2n+9</t>
-  </si>
-  <si>
-    <t>4a+2=7a−22</t>
-  </si>
-  <si>
-    <t>4w−6=3w−1</t>
-  </si>
-  <si>
     <t>3a+5=9a−13</t>
   </si>
   <si>
@@ -172,19 +94,85 @@
   </si>
   <si>
     <t>2d−5=13d−82</t>
+  </si>
+  <si>
+    <t>WAI LUN</t>
+  </si>
+  <si>
+    <t>DONAVAN</t>
+  </si>
+  <si>
+    <t>EILEEN</t>
+  </si>
+  <si>
+    <t>ELICIA</t>
+  </si>
+  <si>
+    <t>JUSTIN</t>
+  </si>
+  <si>
+    <t>JOLIE</t>
+  </si>
+  <si>
+    <t>KELLY</t>
+  </si>
+  <si>
+    <t>ROJEAN</t>
+  </si>
+  <si>
+    <t>DING YANG</t>
+  </si>
+  <si>
+    <t>MANDY</t>
+  </si>
+  <si>
+    <t>SYAKIR</t>
+  </si>
+  <si>
+    <t>RAQIB</t>
+  </si>
+  <si>
+    <t>LATIFAH</t>
+  </si>
+  <si>
+    <t>PATRICK</t>
+  </si>
+  <si>
+    <t>PHIL</t>
+  </si>
+  <si>
+    <t>RUSSELL</t>
+  </si>
+  <si>
+    <t>HAO JUN</t>
+  </si>
+  <si>
+    <t>EVAN</t>
+  </si>
+  <si>
+    <t>NAQIUDDIN</t>
+  </si>
+  <si>
+    <t>YAN KAI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,9 +210,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
@@ -545,7 +537,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,188 +547,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
+      <c r="A1" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
+      <c r="A2" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
+      <c r="A3" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
+      <c r="A4" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
+      <c r="A5" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
+      <c r="A6" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
+      <c r="A7" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
+      <c r="A8" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
+      <c r="A9" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
+      <c r="A10" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
+      <c r="A11" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
+      <c r="A12" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
+      <c r="A13" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
+      <c r="A14" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
+      <c r="A15" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
+      <c r="A16" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
+      <c r="A17" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>31</v>
+      <c r="A18" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
+      <c r="A19" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
+      <c r="A20" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
+      <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" t="s">
-        <v>38</v>
-      </c>
+      <c r="A23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>